<commit_message>
Changed column headers so Matlab creates axis labels without subscripts
</commit_message>
<xml_diff>
--- a/AllPlayerStats.xlsx
+++ b/AllPlayerStats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelsommerfeld/Desktop/Basketball/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1998BB-0C3A-F64F-B4CF-9EF4054100AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73320452-6C87-1D43-9A9E-D133D188E56A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21580" windowHeight="11620" xr2:uid="{C993A551-CEA8-484A-9A43-153B090AB372}"/>
   </bookViews>
@@ -30,18 +30,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>alpha_full_speed</t>
-  </si>
-  <si>
-    <t>AVG_Speed</t>
-  </si>
-  <si>
-    <t>SD_Speed</t>
-  </si>
-  <si>
-    <t>player_number</t>
-  </si>
-  <si>
     <t>Position</t>
   </si>
   <si>
@@ -51,16 +39,10 @@
     <t>FGA</t>
   </si>
   <si>
-    <t>FG%</t>
-  </si>
-  <si>
     <t>3PT</t>
   </si>
   <si>
     <t>3PTA</t>
-  </si>
-  <si>
-    <t>3PT%</t>
   </si>
   <si>
     <t>FT</t>
@@ -69,25 +51,10 @@
     <t>FTA</t>
   </si>
   <si>
-    <t>FT%</t>
-  </si>
-  <si>
-    <t>EFG%</t>
-  </si>
-  <si>
-    <t>TS%</t>
-  </si>
-  <si>
     <t>PTS</t>
   </si>
   <si>
     <t>REB</t>
-  </si>
-  <si>
-    <t>OFF_REB</t>
-  </si>
-  <si>
-    <t>DEF_REB</t>
   </si>
   <si>
     <t>AST</t>
@@ -147,25 +114,58 @@
     <t>Second Half DFA</t>
   </si>
   <si>
-    <t>full_AVG_area</t>
+    <t>Team</t>
   </si>
   <si>
-    <t>full_SD_area</t>
+    <t>full AVG area</t>
   </si>
   <si>
-    <t>first_half_AVG_area</t>
+    <t>full SD area</t>
   </si>
   <si>
-    <t>first_half_SD_area</t>
+    <t>first half AVG area</t>
   </si>
   <si>
-    <t>second_half_AVG_area</t>
+    <t>first half SD area</t>
   </si>
   <si>
-    <t>second_half_SD_area</t>
+    <t>second half AVG area</t>
   </si>
   <si>
-    <t>Team</t>
+    <t>second half SD area</t>
+  </si>
+  <si>
+    <t>alpha full speed</t>
+  </si>
+  <si>
+    <t>AVG Speed</t>
+  </si>
+  <si>
+    <t>SD Speed</t>
+  </si>
+  <si>
+    <t>player number</t>
+  </si>
+  <si>
+    <t>OFF REB</t>
+  </si>
+  <si>
+    <t>DEF REB</t>
+  </si>
+  <si>
+    <t>FG PERC</t>
+  </si>
+  <si>
+    <t>3PT PERC</t>
+  </si>
+  <si>
+    <t>FT PERC</t>
+  </si>
+  <si>
+    <t>EFG PERC</t>
+  </si>
+  <si>
+    <t>TS PERC</t>
   </si>
 </sst>
 </file>
@@ -520,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E87E20B9-AEC1-415A-9E6E-83290650FCD8}">
   <dimension ref="A1:AN209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -542,124 +542,124 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" t="s">
         <v>34</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" t="s">
+      <c r="N1" t="s">
         <v>38</v>
       </c>
-      <c r="E1" t="s">
+      <c r="O1" t="s">
         <v>39</v>
       </c>
-      <c r="F1" t="s">
+      <c r="P1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U1" t="s">
+        <v>42</v>
+      </c>
+      <c r="V1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF1" t="s">
         <v>40</v>
       </c>
-      <c r="G1" t="s">
+      <c r="AG1" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
-        <v>43</v>
-      </c>
-      <c r="J1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
-      </c>
-      <c r="M1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N1" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" t="s">
-        <v>8</v>
-      </c>
-      <c r="V1" t="s">
-        <v>9</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="AH1" t="s">
         <v>10</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AI1" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AJ1" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AK1" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AL1" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AM1" t="s">
         <v>15</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AN1" t="s">
         <v>16</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.2">
@@ -709,7 +709,7 @@
         <v>88</v>
       </c>
       <c r="P2" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -831,7 +831,7 @@
         <v>33</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -953,7 +953,7 @@
         <v>94</v>
       </c>
       <c r="P4" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -1075,7 +1075,7 @@
         <v>87</v>
       </c>
       <c r="P5" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="P6" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -1319,7 +1319,7 @@
         <v>8</v>
       </c>
       <c r="P7" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q7">
         <v>1</v>
@@ -1441,7 +1441,7 @@
         <v>52</v>
       </c>
       <c r="P8" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -1563,7 +1563,7 @@
         <v>6</v>
       </c>
       <c r="P9" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1685,7 +1685,7 @@
         <v>13</v>
       </c>
       <c r="P10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1807,7 +1807,7 @@
         <v>43</v>
       </c>
       <c r="P11" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1929,7 +1929,7 @@
         <v>85</v>
       </c>
       <c r="P12" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q12">
         <v>0</v>
@@ -2051,7 +2051,7 @@
         <v>17</v>
       </c>
       <c r="P13" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q13">
         <v>0</v>
@@ -2173,7 +2173,7 @@
         <v>44</v>
       </c>
       <c r="P14" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -2295,7 +2295,7 @@
         <v>24</v>
       </c>
       <c r="P15" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -2417,7 +2417,7 @@
         <v>25</v>
       </c>
       <c r="P16" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q16">
         <v>0</v>
@@ -2539,7 +2539,7 @@
         <v>81</v>
       </c>
       <c r="P17" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q17">
         <v>0</v>
@@ -2661,7 +2661,7 @@
         <v>75</v>
       </c>
       <c r="P18" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -2783,7 +2783,7 @@
         <v>65</v>
       </c>
       <c r="P19" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2905,7 +2905,7 @@
         <v>51</v>
       </c>
       <c r="P20" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q20">
         <v>0</v>
@@ -3027,7 +3027,7 @@
         <v>113</v>
       </c>
       <c r="P21" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q21">
         <v>0</v>
@@ -3149,7 +3149,7 @@
         <v>110</v>
       </c>
       <c r="P22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q22">
         <v>0</v>
@@ -3271,7 +3271,7 @@
         <v>107</v>
       </c>
       <c r="P23" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q23">
         <v>0</v>
@@ -3393,7 +3393,7 @@
         <v>116</v>
       </c>
       <c r="P24" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q24">
         <v>0</v>
@@ -3515,7 +3515,7 @@
         <v>117</v>
       </c>
       <c r="P25" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q25">
         <v>0</v>
@@ -3637,7 +3637,7 @@
         <v>114</v>
       </c>
       <c r="P26" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q26">
         <v>0</v>
@@ -3759,7 +3759,7 @@
         <v>115</v>
       </c>
       <c r="P27" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q27">
         <v>0</v>
@@ -3881,7 +3881,7 @@
         <v>111</v>
       </c>
       <c r="P28" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -4003,7 +4003,7 @@
         <v>108</v>
       </c>
       <c r="P29" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q29">
         <v>0</v>
@@ -4125,7 +4125,7 @@
         <v>112</v>
       </c>
       <c r="P30" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -4247,7 +4247,7 @@
         <v>106</v>
       </c>
       <c r="P31" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q31">
         <v>0</v>
@@ -4369,7 +4369,7 @@
         <v>90</v>
       </c>
       <c r="P32" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q32">
         <v>0</v>
@@ -4491,7 +4491,7 @@
         <v>99</v>
       </c>
       <c r="P33" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q33">
         <v>0</v>
@@ -4613,7 +4613,7 @@
         <v>109</v>
       </c>
       <c r="P34" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q34">
         <v>0</v>
@@ -4735,7 +4735,7 @@
         <v>12</v>
       </c>
       <c r="P35" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q35">
         <v>1</v>
@@ -4857,7 +4857,7 @@
         <v>56</v>
       </c>
       <c r="P36" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q36">
         <v>1</v>
@@ -4979,7 +4979,7 @@
         <v>53</v>
       </c>
       <c r="P37" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q37">
         <v>1</v>
@@ -5101,7 +5101,7 @@
         <v>28</v>
       </c>
       <c r="P38" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q38">
         <v>1</v>
@@ -5223,7 +5223,7 @@
         <v>78</v>
       </c>
       <c r="P39" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q39">
         <v>1</v>
@@ -5345,7 +5345,7 @@
         <v>70</v>
       </c>
       <c r="P40" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q40">
         <v>1</v>
@@ -5467,7 +5467,7 @@
         <v>10</v>
       </c>
       <c r="P41" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q41">
         <v>1</v>
@@ -5589,7 +5589,7 @@
         <v>66</v>
       </c>
       <c r="P42" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q42">
         <v>1</v>
@@ -5711,7 +5711,7 @@
         <v>124</v>
       </c>
       <c r="P43" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q43">
         <v>1</v>
@@ -5833,7 +5833,7 @@
         <v>98</v>
       </c>
       <c r="P44" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q44">
         <v>1</v>
@@ -5955,7 +5955,7 @@
         <v>55</v>
       </c>
       <c r="P45" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q45">
         <v>1</v>
@@ -6077,7 +6077,7 @@
         <v>27</v>
       </c>
       <c r="P46" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q46">
         <v>1</v>
@@ -6199,7 +6199,7 @@
         <v>20</v>
       </c>
       <c r="P47" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q47">
         <v>1</v>
@@ -6321,7 +6321,7 @@
         <v>47</v>
       </c>
       <c r="P48" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q48">
         <v>1</v>
@@ -6443,7 +6443,7 @@
         <v>97</v>
       </c>
       <c r="P49" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q49">
         <v>1</v>
@@ -6565,7 +6565,7 @@
         <v>22</v>
       </c>
       <c r="P50" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q50">
         <v>1</v>
@@ -6687,7 +6687,7 @@
         <v>84</v>
       </c>
       <c r="P51" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q51">
         <v>1</v>
@@ -6809,7 +6809,7 @@
         <v>2</v>
       </c>
       <c r="P52" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q52">
         <v>1</v>
@@ -6931,7 +6931,7 @@
         <v>38</v>
       </c>
       <c r="P53" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q53">
         <v>1</v>
@@ -7053,7 +7053,7 @@
         <v>50</v>
       </c>
       <c r="P54" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q54">
         <v>1</v>
@@ -7175,7 +7175,7 @@
         <v>45</v>
       </c>
       <c r="P55" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q55">
         <v>1</v>
@@ -7297,7 +7297,7 @@
         <v>91</v>
       </c>
       <c r="P56" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q56">
         <v>1</v>
@@ -7419,7 +7419,7 @@
         <v>33</v>
       </c>
       <c r="P57" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q57">
         <v>1</v>
@@ -7541,7 +7541,7 @@
         <v>74</v>
       </c>
       <c r="P58" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q58">
         <v>0</v>
@@ -7663,7 +7663,7 @@
         <v>69</v>
       </c>
       <c r="P59" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q59">
         <v>0</v>
@@ -7785,7 +7785,7 @@
         <v>21</v>
       </c>
       <c r="P60" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q60">
         <v>0</v>
@@ -7907,7 +7907,7 @@
         <v>32</v>
       </c>
       <c r="P61" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q61">
         <v>0</v>
@@ -8029,7 +8029,7 @@
         <v>57</v>
       </c>
       <c r="P62" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q62">
         <v>0</v>
@@ -8151,7 +8151,7 @@
         <v>11</v>
       </c>
       <c r="P63" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q63">
         <v>0</v>
@@ -8273,7 +8273,7 @@
         <v>95</v>
       </c>
       <c r="P64" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q64">
         <v>0</v>
@@ -8395,7 +8395,7 @@
         <v>37</v>
       </c>
       <c r="P65" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q65">
         <v>0</v>
@@ -8517,7 +8517,7 @@
         <v>73</v>
       </c>
       <c r="P66" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q66">
         <v>0</v>
@@ -8639,7 +8639,7 @@
         <v>42</v>
       </c>
       <c r="P67" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q67">
         <v>0</v>
@@ -8761,7 +8761,7 @@
         <v>113</v>
       </c>
       <c r="P68" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q68">
         <v>0</v>
@@ -8883,7 +8883,7 @@
         <v>110</v>
       </c>
       <c r="P69" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q69">
         <v>0</v>
@@ -9005,7 +9005,7 @@
         <v>107</v>
       </c>
       <c r="P70" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q70">
         <v>0</v>
@@ -9127,7 +9127,7 @@
         <v>116</v>
       </c>
       <c r="P71" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q71">
         <v>0</v>
@@ -9249,7 +9249,7 @@
         <v>117</v>
       </c>
       <c r="P72" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q72">
         <v>0</v>
@@ -9371,7 +9371,7 @@
         <v>114</v>
       </c>
       <c r="P73" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q73">
         <v>0</v>
@@ -9493,7 +9493,7 @@
         <v>115</v>
       </c>
       <c r="P74" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q74">
         <v>0</v>
@@ -9615,7 +9615,7 @@
         <v>111</v>
       </c>
       <c r="P75" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q75">
         <v>0</v>
@@ -9737,7 +9737,7 @@
         <v>108</v>
       </c>
       <c r="P76" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q76">
         <v>0</v>
@@ -9859,7 +9859,7 @@
         <v>112</v>
       </c>
       <c r="P77" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q77">
         <v>0</v>
@@ -9981,7 +9981,7 @@
         <v>106</v>
       </c>
       <c r="P78" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q78">
         <v>0</v>
@@ -10103,7 +10103,7 @@
         <v>90</v>
       </c>
       <c r="P79" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q79">
         <v>0</v>
@@ -10225,7 +10225,7 @@
         <v>99</v>
       </c>
       <c r="P80" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q80">
         <v>0</v>
@@ -10347,7 +10347,7 @@
         <v>109</v>
       </c>
       <c r="P81" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q81">
         <v>0</v>
@@ -10469,7 +10469,7 @@
         <v>39</v>
       </c>
       <c r="P82" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q82">
         <v>1</v>
@@ -10591,7 +10591,7 @@
         <v>83</v>
       </c>
       <c r="P83" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q83">
         <v>1</v>
@@ -10713,7 +10713,7 @@
         <v>89</v>
       </c>
       <c r="P84" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q84">
         <v>1</v>
@@ -10835,7 +10835,7 @@
         <v>5</v>
       </c>
       <c r="P85" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q85">
         <v>1</v>
@@ -10957,7 +10957,7 @@
         <v>96</v>
       </c>
       <c r="P86" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q86">
         <v>1</v>
@@ -11079,7 +11079,7 @@
         <v>30</v>
       </c>
       <c r="P87" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q87">
         <v>1</v>
@@ -11201,7 +11201,7 @@
         <v>63</v>
       </c>
       <c r="P88" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q88">
         <v>1</v>
@@ -11323,7 +11323,7 @@
         <v>71</v>
       </c>
       <c r="P89" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q89">
         <v>1</v>
@@ -11445,7 +11445,7 @@
         <v>35</v>
       </c>
       <c r="P90" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q90">
         <v>1</v>
@@ -11567,7 +11567,7 @@
         <v>62</v>
       </c>
       <c r="P91" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q91">
         <v>1</v>
@@ -11689,7 +11689,7 @@
         <v>14</v>
       </c>
       <c r="P92" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q92">
         <v>1</v>
@@ -11811,7 +11811,7 @@
         <v>88</v>
       </c>
       <c r="P93" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q93">
         <v>1</v>
@@ -11933,7 +11933,7 @@
         <v>33</v>
       </c>
       <c r="P94" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q94">
         <v>1</v>
@@ -12055,7 +12055,7 @@
         <v>94</v>
       </c>
       <c r="P95" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q95">
         <v>1</v>
@@ -12177,7 +12177,7 @@
         <v>87</v>
       </c>
       <c r="P96" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q96">
         <v>1</v>
@@ -12299,7 +12299,7 @@
         <v>49</v>
       </c>
       <c r="P97" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q97">
         <v>1</v>
@@ -12421,7 +12421,7 @@
         <v>31</v>
       </c>
       <c r="P98" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q98">
         <v>1</v>
@@ -12543,7 +12543,7 @@
         <v>8</v>
       </c>
       <c r="P99" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q99">
         <v>1</v>
@@ -12665,7 +12665,7 @@
         <v>52</v>
       </c>
       <c r="P100" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="Q100">
         <v>1</v>
@@ -12787,7 +12787,7 @@
         <v>6</v>
       </c>
       <c r="P101" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q101">
         <v>1</v>
@@ -12909,7 +12909,7 @@
         <v>13</v>
       </c>
       <c r="P102" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q102">
         <v>1</v>
@@ -13031,7 +13031,7 @@
         <v>61</v>
       </c>
       <c r="P103" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q103">
         <v>0</v>
@@ -13153,7 +13153,7 @@
         <v>40</v>
       </c>
       <c r="P104" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q104">
         <v>0</v>
@@ -13275,7 +13275,7 @@
         <v>9</v>
       </c>
       <c r="P105" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q105">
         <v>0</v>
@@ -13397,7 +13397,7 @@
         <v>19</v>
       </c>
       <c r="P106" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q106">
         <v>0</v>
@@ -13519,7 +13519,7 @@
         <v>15</v>
       </c>
       <c r="P107" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q107">
         <v>0</v>
@@ -13641,7 +13641,7 @@
         <v>36</v>
       </c>
       <c r="P108" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q108">
         <v>0</v>
@@ -13763,7 +13763,7 @@
         <v>92</v>
       </c>
       <c r="P109" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q109">
         <v>0</v>
@@ -13885,7 +13885,7 @@
         <v>48</v>
       </c>
       <c r="P110" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q110">
         <v>0</v>
@@ -14007,7 +14007,7 @@
         <v>41</v>
       </c>
       <c r="P111" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q111" s="1">
         <v>0</v>
@@ -14129,7 +14129,7 @@
         <v>55</v>
       </c>
       <c r="P112" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q112" s="1">
         <v>1</v>
@@ -14251,7 +14251,7 @@
         <v>27</v>
       </c>
       <c r="P113" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q113" s="1">
         <v>1</v>
@@ -14373,7 +14373,7 @@
         <v>20</v>
       </c>
       <c r="P114" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q114" s="1">
         <v>1</v>
@@ -14495,7 +14495,7 @@
         <v>47</v>
       </c>
       <c r="P115" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q115" s="1">
         <v>1</v>
@@ -14617,7 +14617,7 @@
         <v>97</v>
       </c>
       <c r="P116" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q116" s="1">
         <v>1</v>
@@ -14739,7 +14739,7 @@
         <v>84</v>
       </c>
       <c r="P117" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q117" s="1">
         <v>1</v>
@@ -14861,7 +14861,7 @@
         <v>2</v>
       </c>
       <c r="P118" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q118" s="1">
         <v>1</v>
@@ -14983,7 +14983,7 @@
         <v>38</v>
       </c>
       <c r="P119" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q119" s="1">
         <v>1</v>
@@ -15105,7 +15105,7 @@
         <v>50</v>
       </c>
       <c r="P120" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q120" s="1">
         <v>1</v>
@@ -15227,7 +15227,7 @@
         <v>45</v>
       </c>
       <c r="P121" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q121" s="1">
         <v>1</v>
@@ -15349,7 +15349,7 @@
         <v>91</v>
       </c>
       <c r="P122" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q122" s="1">
         <v>1</v>
@@ -15471,7 +15471,7 @@
         <v>33</v>
       </c>
       <c r="P123" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q123" s="1">
         <v>1</v>
@@ -15593,7 +15593,7 @@
         <v>3</v>
       </c>
       <c r="P124" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q124" s="1">
         <v>0</v>
@@ -15715,7 +15715,7 @@
         <v>54</v>
       </c>
       <c r="P125" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q125" s="1">
         <v>0</v>
@@ -15837,7 +15837,7 @@
         <v>16</v>
       </c>
       <c r="P126" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q126" s="1">
         <v>0</v>
@@ -15959,7 +15959,7 @@
         <v>60</v>
       </c>
       <c r="P127" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q127" s="1">
         <v>0</v>
@@ -16081,7 +16081,7 @@
         <v>34</v>
       </c>
       <c r="P128" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q128" s="1">
         <v>0</v>
@@ -16203,7 +16203,7 @@
         <v>79</v>
       </c>
       <c r="P129" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q129" s="1">
         <v>0</v>
@@ -16325,7 +16325,7 @@
         <v>86</v>
       </c>
       <c r="P130" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q130" s="1">
         <v>0</v>
@@ -16447,7 +16447,7 @@
         <v>4</v>
       </c>
       <c r="P131" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q131" s="1">
         <v>0</v>
@@ -16569,7 +16569,7 @@
         <v>26</v>
       </c>
       <c r="P132" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q132" s="1">
         <v>0</v>
@@ -16691,7 +16691,7 @@
         <v>64</v>
       </c>
       <c r="P133" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q133" s="1">
         <v>0</v>
@@ -16813,7 +16813,7 @@
         <v>93</v>
       </c>
       <c r="P134" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q134" s="1">
         <v>0</v>
@@ -16935,7 +16935,7 @@
         <v>29</v>
       </c>
       <c r="P135" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q135">
         <v>0</v>
@@ -17057,7 +17057,7 @@
         <v>120</v>
       </c>
       <c r="P136" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q136">
         <v>0</v>
@@ -17179,7 +17179,7 @@
         <v>118</v>
       </c>
       <c r="P137" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q137">
         <v>0</v>
@@ -17301,7 +17301,7 @@
         <v>80</v>
       </c>
       <c r="P138" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q138">
         <v>0</v>
@@ -17423,7 +17423,7 @@
         <v>77</v>
       </c>
       <c r="P139" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q139">
         <v>0</v>
@@ -17545,7 +17545,7 @@
         <v>58</v>
       </c>
       <c r="P140" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q140">
         <v>0</v>
@@ -17667,7 +17667,7 @@
         <v>72</v>
       </c>
       <c r="P141" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q141">
         <v>0</v>
@@ -17789,7 +17789,7 @@
         <v>7</v>
       </c>
       <c r="P142" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q142">
         <v>0</v>
@@ -17911,7 +17911,7 @@
         <v>119</v>
       </c>
       <c r="P143" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q143">
         <v>0</v>
@@ -18033,7 +18033,7 @@
         <v>76</v>
       </c>
       <c r="P144" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q144">
         <v>0</v>
@@ -18155,7 +18155,7 @@
         <v>59</v>
       </c>
       <c r="P145" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q145">
         <v>0</v>
@@ -18277,7 +18277,7 @@
         <v>95</v>
       </c>
       <c r="P146" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q146">
         <v>1</v>
@@ -18399,7 +18399,7 @@
         <v>57</v>
       </c>
       <c r="P147" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q147">
         <v>1</v>
@@ -18521,7 +18521,7 @@
         <v>42</v>
       </c>
       <c r="P148" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q148">
         <v>1</v>
@@ -18643,7 +18643,7 @@
         <v>69</v>
       </c>
       <c r="P149" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q149">
         <v>1</v>
@@ -18765,7 +18765,7 @@
         <v>73</v>
       </c>
       <c r="P150" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q150">
         <v>1</v>
@@ -18887,7 +18887,7 @@
         <v>37</v>
       </c>
       <c r="P151" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q151">
         <v>1</v>
@@ -19009,7 +19009,7 @@
         <v>21</v>
       </c>
       <c r="P152" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q152">
         <v>1</v>
@@ -19131,7 +19131,7 @@
         <v>11</v>
       </c>
       <c r="P153" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q153">
         <v>1</v>
@@ -19253,7 +19253,7 @@
         <v>32</v>
       </c>
       <c r="P154" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q154">
         <v>1</v>
@@ -19375,7 +19375,7 @@
         <v>14</v>
       </c>
       <c r="P155" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q155">
         <v>1</v>
@@ -19497,7 +19497,7 @@
         <v>88</v>
       </c>
       <c r="P156" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q156">
         <v>1</v>
@@ -19619,7 +19619,7 @@
         <v>94</v>
       </c>
       <c r="P157" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q157">
         <v>1</v>
@@ -19741,7 +19741,7 @@
         <v>87</v>
       </c>
       <c r="P158" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q158">
         <v>1</v>
@@ -19863,7 +19863,7 @@
         <v>49</v>
       </c>
       <c r="P159" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q159">
         <v>1</v>
@@ -19985,7 +19985,7 @@
         <v>8</v>
       </c>
       <c r="P160" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q160">
         <v>1</v>
@@ -20107,7 +20107,7 @@
         <v>52</v>
       </c>
       <c r="P161" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="Q161">
         <v>1</v>
@@ -20229,7 +20229,7 @@
         <v>33</v>
       </c>
       <c r="P162" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q162">
         <v>1</v>
@@ -20351,7 +20351,7 @@
         <v>6</v>
       </c>
       <c r="P163" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q163">
         <v>1</v>
@@ -20473,7 +20473,7 @@
         <v>13</v>
       </c>
       <c r="P164" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q164">
         <v>1</v>
@@ -20595,7 +20595,7 @@
         <v>16</v>
       </c>
       <c r="P165" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q165">
         <v>0</v>
@@ -20717,7 +20717,7 @@
         <v>3</v>
       </c>
       <c r="P166" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q166">
         <v>0</v>
@@ -20839,7 +20839,7 @@
         <v>34</v>
       </c>
       <c r="P167" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q167">
         <v>0</v>
@@ -20961,7 +20961,7 @@
         <v>60</v>
       </c>
       <c r="P168" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q168">
         <v>0</v>
@@ -21083,7 +21083,7 @@
         <v>54</v>
       </c>
       <c r="P169" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q169">
         <v>0</v>
@@ -21205,7 +21205,7 @@
         <v>79</v>
       </c>
       <c r="P170" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q170">
         <v>0</v>
@@ -21327,7 +21327,7 @@
         <v>64</v>
       </c>
       <c r="P171" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q171">
         <v>0</v>
@@ -21449,7 +21449,7 @@
         <v>26</v>
       </c>
       <c r="P172" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q172">
         <v>0</v>
@@ -21571,7 +21571,7 @@
         <v>73</v>
       </c>
       <c r="P173" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q173">
         <v>1</v>
@@ -21693,7 +21693,7 @@
         <v>54</v>
       </c>
       <c r="P174" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q174">
         <v>1</v>
@@ -21815,7 +21815,7 @@
         <v>37</v>
       </c>
       <c r="P175" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q175">
         <v>1</v>
@@ -21937,7 +21937,7 @@
         <v>64</v>
       </c>
       <c r="P176" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q176">
         <v>1</v>
@@ -22059,7 +22059,7 @@
         <v>42</v>
       </c>
       <c r="P177" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q177">
         <v>1</v>
@@ -22181,7 +22181,7 @@
         <v>79</v>
       </c>
       <c r="P178" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q178">
         <v>1</v>
@@ -22303,7 +22303,7 @@
         <v>60</v>
       </c>
       <c r="P179" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q179">
         <v>1</v>
@@ -22425,7 +22425,7 @@
         <v>95</v>
       </c>
       <c r="P180" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q180">
         <v>1</v>
@@ -22547,7 +22547,7 @@
         <v>3</v>
       </c>
       <c r="P181" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q181">
         <v>1</v>
@@ -22669,7 +22669,7 @@
         <v>53</v>
       </c>
       <c r="P182" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q182">
         <v>0</v>
@@ -22791,7 +22791,7 @@
         <v>28</v>
       </c>
       <c r="P183" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q183">
         <v>0</v>
@@ -22913,7 +22913,7 @@
         <v>78</v>
       </c>
       <c r="P184" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q184">
         <v>0</v>
@@ -23035,7 +23035,7 @@
         <v>70</v>
       </c>
       <c r="P185" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q185">
         <v>0</v>
@@ -23157,7 +23157,7 @@
         <v>10</v>
       </c>
       <c r="P186" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q186">
         <v>0</v>
@@ -23279,7 +23279,7 @@
         <v>12</v>
       </c>
       <c r="P187" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q187">
         <v>0</v>
@@ -23401,7 +23401,7 @@
         <v>124</v>
       </c>
       <c r="P188" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q188">
         <v>0</v>
@@ -23523,7 +23523,7 @@
         <v>66</v>
       </c>
       <c r="P189" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q189">
         <v>0</v>
@@ -23645,7 +23645,7 @@
         <v>47</v>
       </c>
       <c r="P190" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q190">
         <v>0</v>
@@ -23767,7 +23767,7 @@
         <v>55</v>
       </c>
       <c r="P191" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q191">
         <v>0</v>
@@ -23889,7 +23889,7 @@
         <v>27</v>
       </c>
       <c r="P192" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q192">
         <v>0</v>
@@ -24011,7 +24011,7 @@
         <v>84</v>
       </c>
       <c r="P193" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q193">
         <v>0</v>
@@ -24133,7 +24133,7 @@
         <v>22</v>
       </c>
       <c r="P194" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q194">
         <v>0</v>
@@ -24255,7 +24255,7 @@
         <v>38</v>
       </c>
       <c r="P195" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q195">
         <v>0</v>
@@ -24377,7 +24377,7 @@
         <v>20</v>
       </c>
       <c r="P196" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q196">
         <v>0</v>
@@ -24499,7 +24499,7 @@
         <v>50</v>
       </c>
       <c r="P197" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q197">
         <v>0</v>
@@ -24621,7 +24621,7 @@
         <v>33</v>
       </c>
       <c r="P198" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q198">
         <v>0</v>
@@ -24743,7 +24743,7 @@
         <v>97</v>
       </c>
       <c r="P199" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q199">
         <v>0</v>
@@ -24865,7 +24865,7 @@
         <v>2</v>
       </c>
       <c r="P200" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q200">
         <v>0</v>
@@ -24987,7 +24987,7 @@
         <v>64</v>
       </c>
       <c r="P201" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q201">
         <v>1</v>
@@ -25109,7 +25109,7 @@
         <v>3</v>
       </c>
       <c r="P202" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="Q202">
         <v>1</v>
@@ -25231,7 +25231,7 @@
         <v>54</v>
       </c>
       <c r="P203" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q203">
         <v>1</v>
@@ -25353,7 +25353,7 @@
         <v>16</v>
       </c>
       <c r="P204" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="Q204">
         <v>1</v>
@@ -25475,7 +25475,7 @@
         <v>60</v>
       </c>
       <c r="P205" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="Q205">
         <v>1</v>
@@ -25597,7 +25597,7 @@
         <v>34</v>
       </c>
       <c r="P206" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q206">
         <v>1</v>
@@ -25719,7 +25719,7 @@
         <v>79</v>
       </c>
       <c r="P207" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="Q207">
         <v>1</v>
@@ -25841,7 +25841,7 @@
         <v>86</v>
       </c>
       <c r="P208" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q208">
         <v>1</v>
@@ -25963,7 +25963,7 @@
         <v>4</v>
       </c>
       <c r="P209" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="Q209">
         <v>1</v>
@@ -26044,21 +26044,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006AD42462C90CFD4E9778A3BCE30090F0" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="29e91910654a4bcbf5597f8144de98c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4cd45121-ea8f-4099-aeaf-67ab6e28b8bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cc5fe2d8c58b5a865e13c362f1430e42" ns2:_="">
     <xsd:import namespace="4cd45121-ea8f-4099-aeaf-67ab6e28b8bf"/>
@@ -26204,24 +26189,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C052E266-E0E7-4618-9FD1-D77A11628858}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E56EA09-5AE7-4D21-B6B8-079EA7A7E377}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7611B6A8-D666-4C4B-A167-BE2E851030C1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -26237,4 +26220,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E56EA09-5AE7-4D21-B6B8-079EA7A7E377}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C052E266-E0E7-4618-9FD1-D77A11628858}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>